<commit_message>
Uploaded 06-Jun-2022 20:54:16 {/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx
+++ b/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx
@@ -516,7 +516,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -713,7 +713,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="F14" s="10">
         <v>5</v>

</xml_diff>

<commit_message>
Uploaded 07-Jun-2022 14:46:41 {/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx
+++ b/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx
@@ -61,9 +61,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>20,60</t>
-  </si>
-  <si>
     <t>ACTION</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   <si>
     <t>orderDiscount.setDiscount(orderDiscount.getDiscount() + $param);
 System.out.println("Applying discount of "+$param+"% for customer "+orderRequest.getCustomerNumber());</t>
+  </si>
+  <si>
+    <t>20,50</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -546,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -555,7 +555,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -612,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -628,19 +628,19 @@
     <row r="9" spans="1:6" ht="75">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -651,16 +651,16 @@
         <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="F10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -668,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -683,7 +683,7 @@
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -698,7 +698,7 @@
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="10">
@@ -713,7 +713,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="F14" s="10">
         <v>5</v>

</xml_diff>

<commit_message>
Uploaded 08-Jun-2022 19:51:00 {/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx
+++ b/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx
@@ -98,7 +98,7 @@
 System.out.println("Applying discount of "+$param+"% for customer "+orderRequest.getCustomerNumber());</t>
   </si>
   <si>
-    <t>20,50</t>
+    <t>20,60</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Uploaded 23-Jun-2022 16:26:27 {/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx
+++ b/src/main/resources/com/jazz/drools/Order_discount_rules.xlsx
@@ -516,7 +516,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -713,7 +713,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="F14" s="10">
         <v>5</v>

</xml_diff>